<commit_message>
populate db from a spreadsheet
</commit_message>
<xml_diff>
--- a/researchPlannerData.xlsx
+++ b/researchPlannerData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Shillitoe\source\repos\research_planner_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33E19D-362D-4697-B70A-5517D3C9AFA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE8EC8-CBEF-449A-9831-0A53382AB098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990" activeTab="1" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="Patient" sheetId="2" r:id="rId2"/>
+    <sheet name="Patients" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,9 +61,6 @@
     <t>There must be a header row</t>
   </si>
   <si>
-    <t>This tab must be called 'Patient'</t>
-  </si>
-  <si>
     <t>This tab must be called 'Tasks'</t>
   </si>
   <si>
@@ -92,6 +89,9 @@
   </si>
   <si>
     <t>Task 7</t>
+  </si>
+  <si>
+    <t>This tab must be called 'Patients'</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED7451-5C9C-419F-8F41-C05A64185FAF}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -504,21 +504,21 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <v>2</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
@@ -566,7 +566,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3">
         <v>3</v>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840549CD-C66E-46CE-91B1-DDF72DBA04B1}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,7 +600,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
added id field to Tasks table
</commit_message>
<xml_diff>
--- a/researchPlannerData.xlsx
+++ b/researchPlannerData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Shillitoe\source\repos\research_planner_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBE8EC8-CBEF-449A-9831-0A53382AB098}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D420ED0-08D0-44E8-A78B-8A8D6BD546F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990" activeTab="1" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Patient 0001</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>This tab must be called 'Patients'</t>
+  </si>
+  <si>
+    <t>Kidney Volumes</t>
+  </si>
+  <si>
+    <t>Patient 0009</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>Patient 0010</t>
+  </si>
+  <si>
+    <t>iBeat 0001</t>
   </si>
 </sst>
 </file>
@@ -136,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -159,17 +174,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ED7451-5C9C-419F-8F41-C05A64185FAF}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,7 +551,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -529,7 +559,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -545,7 +575,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -553,7 +583,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -561,7 +591,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -569,6 +599,22 @@
         <v>20</v>
       </c>
       <c r="B8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5">
         <v>3</v>
       </c>
     </row>
@@ -580,10 +626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840549CD-C66E-46CE-91B1-DDF72DBA04B1}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -643,6 +689,21 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated data input file
</commit_message>
<xml_diff>
--- a/researchPlannerData.xlsx
+++ b/researchPlannerData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steve Shillitoe\source\repos\research_planner_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sshil\source\repos\research_planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D420ED0-08D0-44E8-A78B-8A8D6BD546F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2974408-5388-43AA-809E-FBE0DA77FFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5990" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4A0F660A-41FA-43B1-8018-D8F8F17A55F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Patient 0001</t>
   </si>
@@ -70,43 +70,37 @@
     <t>Repetitions</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
-    <t>Task 7</t>
-  </si>
-  <si>
     <t>This tab must be called 'Patients'</t>
   </si>
   <si>
-    <t>Kidney Volumes</t>
-  </si>
-  <si>
     <t>Patient 0009</t>
   </si>
   <si>
-    <t>AAA</t>
-  </si>
-  <si>
     <t>Patient 0010</t>
   </si>
   <si>
     <t>iBeat 0001</t>
+  </si>
+  <si>
+    <t>Kidney Area</t>
+  </si>
+  <si>
+    <t>Liver Area</t>
+  </si>
+  <si>
+    <t>Kidney Vol.</t>
+  </si>
+  <si>
+    <t>Kidney Conc.</t>
+  </si>
+  <si>
+    <t>Liver Vol.</t>
+  </si>
+  <si>
+    <t>Liver Conc.</t>
+  </si>
+  <si>
+    <t>Decay Rate</t>
   </si>
 </sst>
 </file>
@@ -199,7 +193,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,7 +511,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,7 +542,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
@@ -556,7 +550,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -564,7 +558,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -572,7 +566,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -580,7 +574,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
@@ -588,7 +582,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="3">
         <v>3</v>
@@ -596,27 +590,19 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5">
-        <v>2</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5">
-        <v>3</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -646,7 +632,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -691,17 +677,17 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>